<commit_message>
Removed TADS from baseline comparisons Calculated between group effect sizes for psy active vs control
</commit_message>
<xml_diff>
--- a/for_despina_and_giannis_200224.xlsx
+++ b/for_despina_and_giannis_200224.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/rejucbu_ucl_ac_uk/Documents/Response to Psychological and Pharmacological Treatment for Depression in Children and Adolescents/apples_oranges/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlotte\OneDrive - University College London\Response to Psychological and Pharmacological Treatment for Depression in Children and Adolescents\apples_oranges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{973358FA-7BCC-4B6A-B554-2A5ADB6712AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B81BD81-6B6B-408E-9AE2-8C94F7E0F081}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="13_ncr:1_{973358FA-7BCC-4B6A-B554-2A5ADB6712AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{57C16A3E-3842-4240-A6B6-00DBB9682D1D}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1941" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1927" uniqueCount="606">
   <si>
     <t>Y</t>
   </si>
@@ -2615,10 +2615,10 @@
   <dimension ref="A1:AG125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="P122" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="N93" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S123" sqref="S123"/>
+      <selection pane="bottomRight" activeCell="O96" sqref="O96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5"/>
@@ -8330,26 +8330,26 @@
       <c r="H76" t="s">
         <v>31</v>
       </c>
-      <c r="I76" s="13" t="s">
-        <v>32</v>
+      <c r="I76" s="13">
+        <v>0</v>
       </c>
       <c r="J76" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="K76" s="13" t="s">
-        <v>32</v>
+      <c r="K76" s="13">
+        <v>0</v>
       </c>
       <c r="L76" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="M76" s="13" t="s">
-        <v>32</v>
+      <c r="M76" s="13">
+        <v>0</v>
       </c>
       <c r="N76" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="O76" s="18" t="s">
-        <v>32</v>
+      <c r="O76" s="18">
+        <v>0</v>
       </c>
       <c r="P76" s="18" t="s">
         <v>271</v>
@@ -10055,14 +10055,14 @@
       <c r="L96" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="M96" s="13" t="s">
-        <v>32</v>
+      <c r="M96" s="13">
+        <v>0</v>
       </c>
       <c r="N96" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="O96" s="13" t="s">
-        <v>32</v>
+      <c r="O96" s="13">
+        <v>0</v>
       </c>
       <c r="P96" s="13" t="s">
         <v>32</v>
@@ -10577,7 +10577,7 @@
         <v>466</v>
       </c>
       <c r="M102" s="18">
-        <v>130</v>
+        <v>43</v>
       </c>
       <c r="N102" s="18" t="s">
         <v>389</v>
@@ -10822,26 +10822,26 @@
       <c r="H105" t="s">
         <v>40</v>
       </c>
-      <c r="I105" s="13" t="s">
-        <v>32</v>
+      <c r="I105" s="13">
+        <v>0</v>
       </c>
       <c r="J105" s="18" t="s">
         <v>412</v>
       </c>
-      <c r="K105" s="13" t="s">
-        <v>32</v>
+      <c r="K105" s="13">
+        <v>0</v>
       </c>
       <c r="L105" s="19" t="s">
         <v>413</v>
       </c>
-      <c r="M105" s="13" t="s">
-        <v>32</v>
+      <c r="M105" s="13">
+        <v>0</v>
       </c>
       <c r="N105" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="O105" s="13" t="s">
-        <v>32</v>
+      <c r="O105" s="13">
+        <v>0</v>
       </c>
       <c r="P105" s="13" t="s">
         <v>32</v>
@@ -10994,26 +10994,26 @@
       <c r="H107" t="s">
         <v>40</v>
       </c>
-      <c r="I107" s="13" t="s">
-        <v>32</v>
+      <c r="I107" s="13">
+        <v>0</v>
       </c>
       <c r="J107" s="18" t="s">
         <v>428</v>
       </c>
-      <c r="K107" s="13" t="s">
-        <v>32</v>
+      <c r="K107" s="13">
+        <v>0</v>
       </c>
       <c r="L107" s="19" t="s">
         <v>429</v>
       </c>
-      <c r="M107" s="13" t="s">
-        <v>32</v>
+      <c r="M107" s="13">
+        <v>0</v>
       </c>
       <c r="N107" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="O107" s="13" t="s">
-        <v>32</v>
+      <c r="O107" s="13">
+        <v>0</v>
       </c>
       <c r="P107" s="13" t="s">
         <v>32</v>
@@ -12914,20 +12914,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="2fde0613-ae2a-4b9e-9dd8-0a3a1ae5b78b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2fde0613-ae2a-4b9e-9dd8-0a3a1ae5b78b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12950,26 +12950,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C39317AC-9C3F-479D-B1F6-7885FA217E14}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A218EC1-C381-41FC-BD63-A63076232149}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e7bbc584-5a77-4c67-8fd7-7058eeaacc07"/>
-    <ds:schemaRef ds:uri="2fde0613-ae2a-4b9e-9dd8-0a3a1ae5b78b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A218EC1-C381-41FC-BD63-A63076232149}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C39317AC-9C3F-479D-B1F6-7885FA217E14}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="2fde0613-ae2a-4b9e-9dd8-0a3a1ae5b78b"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7bbc584-5a77-4c67-8fd7-7058eeaacc07"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
some changes for revision
</commit_message>
<xml_diff>
--- a/for_despina_and_giannis_200224.xlsx
+++ b/for_despina_and_giannis_200224.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlotte\OneDrive - University College London\Response to Psychological and Pharmacological Treatment for Depression in Children and Adolescents\apples_oranges\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphaelle\Documents\AIM Lab\apples_and_oranges\main_git\apples_oranges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{973358FA-7BCC-4B6A-B554-2A5ADB6712AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{20ECA2EE-CFA1-4ACC-8F3D-87869DA55FBF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12175A4A-22B2-47DC-B0BD-16C61ED9C90D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1927" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2049" uniqueCount="641">
   <si>
     <t>Y</t>
   </si>
@@ -2028,6 +2028,117 @@
   </si>
   <si>
     <t>16</t>
+  </si>
+  <si>
+    <t>Poole, 2017</t>
+  </si>
+  <si>
+    <t>Reed, 1994</t>
+  </si>
+  <si>
+    <t>Shirk, 2014</t>
+  </si>
+  <si>
+    <t>Brent, 1997</t>
+  </si>
+  <si>
+    <t>Poole. 2017</t>
+  </si>
+  <si>
+    <t>behaviour exchange systems therapy</t>
+  </si>
+  <si>
+    <t>Community settings in Melbourne and Geelong, Victoria</t>
+  </si>
+  <si>
+    <t>4 parent only + 4 adolescent and siblings</t>
+  </si>
+  <si>
+    <t>7 parents only + 1 all invited to attend</t>
+  </si>
+  <si>
+    <t>weekly</t>
+  </si>
+  <si>
+    <t>clinical psychologists, registered psychologists or postgraduate clinical psychology trainees with a training workshop of equivalent length and were provided supervision in equal amounts by one of the creators of the intervention, who monitored fidelity to the intervention manual.</t>
+  </si>
+  <si>
+    <t>individual, parents and siblings</t>
+  </si>
+  <si>
+    <t>supervision</t>
+  </si>
+  <si>
+    <t>structured learning therapy</t>
+  </si>
+  <si>
+    <t>art and imagery exercises</t>
+  </si>
+  <si>
+    <t>northwest Ohio</t>
+  </si>
+  <si>
+    <t>biweekly</t>
+  </si>
+  <si>
+    <t>biweekly (not clear if twice a week or every two weeks)</t>
+  </si>
+  <si>
+    <t>not clear if 12 or 6</t>
+  </si>
+  <si>
+    <t>led by two therapists</t>
+  </si>
+  <si>
+    <t>12 adolescents</t>
+  </si>
+  <si>
+    <t>6 adolescents</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> two
+ outpatient clinics of a community mental health center in a large
+ ethnically diverse urban city in the Rocky Mountain west.</t>
+  </si>
+  <si>
+    <t>two
+ female doctoral-level psychologists (with 3 and 4 years of clinical
+ experience, respectively)</t>
+  </si>
+  <si>
+    <t>one male, doctoral-level psychologist with 28 years of
+ clinical experience; one female, masters-level therapist with 10
+ years of experience.</t>
+  </si>
+  <si>
+    <t>adherence checklist</t>
+  </si>
+  <si>
+    <t>systemic behavior family therapy</t>
+  </si>
+  <si>
+    <t>non-directive supportive treatment</t>
+  </si>
+  <si>
+    <t>12 to 16 weeks</t>
+  </si>
+  <si>
+    <t>each therapist had 6 months of intensive training using a cell-specific treatment manual and a library of training videotapes</t>
+  </si>
+  <si>
+    <t>12-16 weeks (hours distributed)</t>
+  </si>
+  <si>
+    <t>12-16 sessions (hours distributed)</t>
+  </si>
+  <si>
+    <t>Treatment credibility (TxC) is a measure derived from Borkovec and Nau</t>
+  </si>
+  <si>
+    <t>supervision and group</t>
   </si>
 </sst>
 </file>
@@ -2219,7 +2330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2298,6 +2409,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2612,19 +2725,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG125"/>
+  <dimension ref="A1:AG134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="G118" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F131" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H117" sqref="H117"/>
+      <selection pane="bottomRight" activeCell="A132" sqref="A132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="3.81640625" customWidth="1"/>
-    <col min="2" max="2" width="3.36328125" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.1796875" customWidth="1"/>
     <col min="5" max="5" width="15.453125" customWidth="1"/>
@@ -12684,6 +12797,518 @@
         <v>32</v>
       </c>
     </row>
+    <row r="126" spans="1:32" ht="145">
+      <c r="A126">
+        <v>57</v>
+      </c>
+      <c r="B126">
+        <v>131</v>
+      </c>
+      <c r="C126" s="13" t="s">
+        <v>606</v>
+      </c>
+      <c r="D126" s="40" t="s">
+        <v>611</v>
+      </c>
+      <c r="E126" t="s">
+        <v>143</v>
+      </c>
+      <c r="F126" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G126" t="s">
+        <v>612</v>
+      </c>
+      <c r="H126" t="s">
+        <v>31</v>
+      </c>
+      <c r="I126" s="13">
+        <v>8</v>
+      </c>
+      <c r="J126" s="13" t="s">
+        <v>613</v>
+      </c>
+      <c r="K126" s="13">
+        <v>1</v>
+      </c>
+      <c r="L126" s="13" t="s">
+        <v>615</v>
+      </c>
+      <c r="M126" s="13">
+        <v>120</v>
+      </c>
+      <c r="O126">
+        <v>16</v>
+      </c>
+      <c r="S126">
+        <v>8</v>
+      </c>
+      <c r="U126" s="5" t="s">
+        <v>616</v>
+      </c>
+      <c r="W126" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="X126" t="s">
+        <v>617</v>
+      </c>
+      <c r="Y126" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z126" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA126" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB126" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC126" s="13" t="s">
+        <v>628</v>
+      </c>
+      <c r="AD126" s="13"/>
+      <c r="AE126" s="13" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="127" spans="1:32">
+      <c r="C127" s="13" t="s">
+        <v>610</v>
+      </c>
+      <c r="D127" t="s">
+        <v>143</v>
+      </c>
+      <c r="F127" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G127" t="s">
+        <v>612</v>
+      </c>
+      <c r="H127" t="s">
+        <v>40</v>
+      </c>
+      <c r="I127" s="13">
+        <v>8</v>
+      </c>
+      <c r="J127" s="13" t="s">
+        <v>614</v>
+      </c>
+      <c r="K127" s="13">
+        <v>1</v>
+      </c>
+      <c r="L127" s="13" t="s">
+        <v>615</v>
+      </c>
+      <c r="M127" s="13">
+        <v>120</v>
+      </c>
+      <c r="O127">
+        <v>16</v>
+      </c>
+      <c r="S127" s="13">
+        <v>8</v>
+      </c>
+      <c r="W127" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="X127" t="s">
+        <v>617</v>
+      </c>
+      <c r="Y127" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z127" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA127" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB127" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC127" s="13" t="s">
+        <v>628</v>
+      </c>
+      <c r="AE127" s="13" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="128" spans="1:32">
+      <c r="C128" s="13" t="s">
+        <v>607</v>
+      </c>
+      <c r="D128" s="40" t="s">
+        <v>619</v>
+      </c>
+      <c r="E128" t="s">
+        <v>127</v>
+      </c>
+      <c r="F128" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G128" t="s">
+        <v>621</v>
+      </c>
+      <c r="H128" t="s">
+        <v>31</v>
+      </c>
+      <c r="I128" s="13">
+        <v>6</v>
+      </c>
+      <c r="K128" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="L128" s="13" t="s">
+        <v>623</v>
+      </c>
+      <c r="M128" s="13">
+        <v>60</v>
+      </c>
+      <c r="O128">
+        <v>6</v>
+      </c>
+      <c r="S128" s="13">
+        <v>12</v>
+      </c>
+      <c r="T128" t="s">
+        <v>624</v>
+      </c>
+      <c r="U128" t="s">
+        <v>625</v>
+      </c>
+      <c r="W128" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="X128" t="s">
+        <v>626</v>
+      </c>
+      <c r="Y128" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA128" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC128" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="AE128" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="129" spans="3:31">
+      <c r="C129" s="13" t="s">
+        <v>607</v>
+      </c>
+      <c r="D129" s="40" t="s">
+        <v>620</v>
+      </c>
+      <c r="E129" t="s">
+        <v>32</v>
+      </c>
+      <c r="F129" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H129" t="s">
+        <v>40</v>
+      </c>
+      <c r="I129" s="13">
+        <v>6</v>
+      </c>
+      <c r="K129" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="L129" s="13" t="s">
+        <v>622</v>
+      </c>
+      <c r="M129" s="13">
+        <v>60</v>
+      </c>
+      <c r="O129">
+        <v>6</v>
+      </c>
+      <c r="S129" s="13">
+        <v>12</v>
+      </c>
+      <c r="T129" t="s">
+        <v>624</v>
+      </c>
+      <c r="U129" t="s">
+        <v>625</v>
+      </c>
+      <c r="W129" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="X129" t="s">
+        <v>627</v>
+      </c>
+      <c r="Y129" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA129" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="130" spans="3:31" ht="72.5">
+      <c r="C130" s="13" t="s">
+        <v>608</v>
+      </c>
+      <c r="D130" s="40" t="s">
+        <v>554</v>
+      </c>
+      <c r="E130" t="s">
+        <v>143</v>
+      </c>
+      <c r="F130">
+        <v>2</v>
+      </c>
+      <c r="G130" s="5" t="s">
+        <v>629</v>
+      </c>
+      <c r="H130" t="s">
+        <v>31</v>
+      </c>
+      <c r="I130" s="13">
+        <v>12</v>
+      </c>
+      <c r="K130" s="13">
+        <v>1</v>
+      </c>
+      <c r="M130" t="s">
+        <v>32</v>
+      </c>
+      <c r="O130" t="s">
+        <v>32</v>
+      </c>
+      <c r="S130" s="13">
+        <v>12</v>
+      </c>
+      <c r="U130" s="5" t="s">
+        <v>631</v>
+      </c>
+      <c r="W130" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y130" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC130" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE130" s="13" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="131" spans="3:31" ht="72.5">
+      <c r="C131" s="13" t="s">
+        <v>608</v>
+      </c>
+      <c r="D131" s="40" t="s">
+        <v>143</v>
+      </c>
+      <c r="E131" t="s">
+        <v>32</v>
+      </c>
+      <c r="F131">
+        <v>2</v>
+      </c>
+      <c r="H131" t="s">
+        <v>40</v>
+      </c>
+      <c r="I131" s="13">
+        <v>12</v>
+      </c>
+      <c r="K131" s="13">
+        <v>1</v>
+      </c>
+      <c r="M131" t="s">
+        <v>32</v>
+      </c>
+      <c r="O131" t="s">
+        <v>32</v>
+      </c>
+      <c r="S131" s="13">
+        <v>12</v>
+      </c>
+      <c r="U131" s="5" t="s">
+        <v>630</v>
+      </c>
+      <c r="W131" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y131" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC131" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE131" s="13"/>
+    </row>
+    <row r="132" spans="3:31" ht="43.5">
+      <c r="C132" s="13" t="s">
+        <v>609</v>
+      </c>
+      <c r="D132" s="40" t="s">
+        <v>554</v>
+      </c>
+      <c r="E132" t="s">
+        <v>143</v>
+      </c>
+      <c r="F132" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H132" t="s">
+        <v>31</v>
+      </c>
+      <c r="I132" s="13">
+        <v>12.1</v>
+      </c>
+      <c r="J132" t="s">
+        <v>638</v>
+      </c>
+      <c r="K132" s="13">
+        <v>1</v>
+      </c>
+      <c r="M132" t="s">
+        <v>32</v>
+      </c>
+      <c r="O132">
+        <v>12.5</v>
+      </c>
+      <c r="S132" s="13">
+        <v>13.9</v>
+      </c>
+      <c r="T132" s="41" t="s">
+        <v>635</v>
+      </c>
+      <c r="U132" t="s">
+        <v>636</v>
+      </c>
+      <c r="W132" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y132" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA132" s="13" t="s">
+        <v>628</v>
+      </c>
+      <c r="AB132" s="5" t="s">
+        <v>639</v>
+      </c>
+      <c r="AC132" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE132" s="13" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="133" spans="3:31">
+      <c r="C133" s="13" t="s">
+        <v>609</v>
+      </c>
+      <c r="D133" s="40" t="s">
+        <v>633</v>
+      </c>
+      <c r="E133" t="s">
+        <v>143</v>
+      </c>
+      <c r="F133" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H133" t="s">
+        <v>31</v>
+      </c>
+      <c r="I133" s="13">
+        <v>10.7</v>
+      </c>
+      <c r="J133" t="s">
+        <v>638</v>
+      </c>
+      <c r="K133" s="13">
+        <v>1</v>
+      </c>
+      <c r="M133" t="s">
+        <v>32</v>
+      </c>
+      <c r="O133">
+        <v>11.7</v>
+      </c>
+      <c r="S133" s="13">
+        <v>12</v>
+      </c>
+      <c r="T133" s="41" t="s">
+        <v>635</v>
+      </c>
+      <c r="W133" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y133" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA133" s="13" t="s">
+        <v>628</v>
+      </c>
+      <c r="AC133" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE133" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="134" spans="3:31">
+      <c r="C134" s="13" t="s">
+        <v>609</v>
+      </c>
+      <c r="D134" s="40" t="s">
+        <v>634</v>
+      </c>
+      <c r="E134" t="s">
+        <v>32</v>
+      </c>
+      <c r="F134" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H134" t="s">
+        <v>40</v>
+      </c>
+      <c r="I134" s="13">
+        <v>11.2</v>
+      </c>
+      <c r="J134" t="s">
+        <v>637</v>
+      </c>
+      <c r="K134" s="13">
+        <v>1</v>
+      </c>
+      <c r="M134" t="s">
+        <v>32</v>
+      </c>
+      <c r="O134">
+        <v>11.6</v>
+      </c>
+      <c r="S134" s="13">
+        <v>12.9</v>
+      </c>
+      <c r="T134" s="41" t="s">
+        <v>635</v>
+      </c>
+      <c r="W134" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y134" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA134" s="13" t="s">
+        <v>628</v>
+      </c>
+      <c r="AC134" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE134" s="13" t="s">
+        <v>640</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="W1:W125" xr:uid="{ED396039-E314-4A59-A18D-7C812E01C643}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12693,6 +13318,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2fde0613-ae2a-4b9e-9dd8-0a3a1ae5b78b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CE7BC97E19D5434CB0B01A1ABCBF2DDD" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e75b4284d528a6b18ce77feafc1e78ac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2fde0613-ae2a-4b9e-9dd8-0a3a1ae5b78b" xmlns:ns4="e7bbc584-5a77-4c67-8fd7-7058eeaacc07" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d1a975e0f863fb9b7e4676b30af5bf6" ns3:_="" ns4:_="">
     <xsd:import namespace="2fde0613-ae2a-4b9e-9dd8-0a3a1ae5b78b"/>
@@ -12919,14 +13552,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="2fde0613-ae2a-4b9e-9dd8-0a3a1ae5b78b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -12937,6 +13562,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C39317AC-9C3F-479D-B1F6-7885FA217E14}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="e7bbc584-5a77-4c67-8fd7-7058eeaacc07"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="2fde0613-ae2a-4b9e-9dd8-0a3a1ae5b78b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFBB7BDA-9D7A-402A-8216-B63182C80A82}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12955,23 +13597,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C39317AC-9C3F-479D-B1F6-7885FA217E14}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="e7bbc584-5a77-4c67-8fd7-7058eeaacc07"/>
-    <ds:schemaRef ds:uri="2fde0613-ae2a-4b9e-9dd8-0a3a1ae5b78b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A218EC1-C381-41FC-BD63-A63076232149}">
   <ds:schemaRefs>

</xml_diff>